<commit_message>
Docker and docker-compose config
</commit_message>
<xml_diff>
--- a/files/estoque.xlsx
+++ b/files/estoque.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
feat: add function to update stock
</commit_message>
<xml_diff>
--- a/files/estoque.xlsx
+++ b/files/estoque.xlsx
@@ -465,7 +465,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -522,7 +522,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="n">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Updated comodoro.py and Cox Comodoro.py
</commit_message>
<xml_diff>
--- a/files/estoque.xlsx
+++ b/files/estoque.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,139 +460,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>aa</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>17.5</v>
-      </c>
-      <c r="E2" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B3" t="n">
-        <v>10</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>bb</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>20</v>
-      </c>
-      <c r="E3" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>cc</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>20</v>
-      </c>
-      <c r="E4" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>46</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>dd</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>50</v>
-      </c>
-      <c r="E5" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B6" t="n">
-        <v>10</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>rrrr</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>17</v>
-      </c>
-      <c r="E6" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" t="n">
-        <v>10</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>local</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>17</v>
-      </c>
-      <c r="E7" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>202</v>
-      </c>
-      <c r="B8" t="n">
-        <v>20</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>peças moto</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>22.9</v>
-      </c>
-      <c r="E8" t="n">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>